<commit_message>
Update summary (windows) max post adj.xlsx
</commit_message>
<xml_diff>
--- a/ForegroundJobScheduler/results/Nonoverlapping windows/summary (windows) max post adj.xlsx
+++ b/ForegroundJobScheduler/results/Nonoverlapping windows/summary (windows) max post adj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\GitHub\Research-Projects\ForegroundJobScheduler\results\Nonoverlapping windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A4DEA-B011-4115-BC95-EC4205B7CEF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEBACB4-A719-44B8-A3B0-2A19EF84AD7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="3684" windowWidth="23040" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10392" yWindow="3972" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,7 +900,7 @@
         <v>0.39090265755734238</v>
       </c>
       <c r="G19">
-        <v>0.9636526594614383</v>
+        <v>0.95556586348402406</v>
       </c>
       <c r="H19">
         <v>0.4435153732253288</v>
@@ -988,6 +988,18 @@
       <c r="E23">
         <v>3000</v>
       </c>
+      <c r="F23">
+        <v>0.43762828849158847</v>
+      </c>
+      <c r="G23">
+        <v>0.94580304031725049</v>
+      </c>
+      <c r="H23">
+        <v>0.45767485526521673</v>
+      </c>
+      <c r="I23">
+        <v>0.67427802363246503</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1068,6 +1080,18 @@
       <c r="E27">
         <v>3000</v>
       </c>
+      <c r="F27">
+        <v>0.48965119649127259</v>
+      </c>
+      <c r="G27">
+        <v>0.93136768293326855</v>
+      </c>
+      <c r="H27">
+        <v>0.48952825654054799</v>
+      </c>
+      <c r="I27">
+        <v>0.67573271833768012</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1147,6 +1171,18 @@
       </c>
       <c r="E31">
         <v>3000</v>
+      </c>
+      <c r="F31">
+        <v>0.63701747803985442</v>
+      </c>
+      <c r="G31">
+        <v>0.86200016207703911</v>
+      </c>
+      <c r="H31">
+        <v>0.59967446907456212</v>
+      </c>
+      <c r="I31">
+        <v>0.68574966538504167</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>